<commit_message>
update excel document and move web api to seperate
</commit_message>
<xml_diff>
--- a/API URLs.xlsx
+++ b/API URLs.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ryan\Documents\Git\ThirdYearProject\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Git\ThirdYearProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -35,16 +35,16 @@
     <t>Description</t>
   </si>
   <si>
-    <t>http://localhost:3688/api/timetable/{id}</t>
-  </si>
-  <si>
     <t>Returns a Json representation of today's timetable for the user specified in {id}</t>
   </si>
   <si>
-    <t>http://localhost:3688/api/Timetables/GetRoomTimeTable?id={roomid}&amp;weekDayNum={weekdayNum}</t>
-  </si>
-  <si>
     <t>Returns a Json representation of the timetable for the room specified in {roomid} for the day specified by {weekdayNum} (1 = Sunday, 2 = Monday, etc.)</t>
+  </si>
+  <si>
+    <t>http://signmeinwebapi.azurewebsites.net/api/timetable/{id}</t>
+  </si>
+  <si>
+    <t>http://signmeinwebapi.azurewebsites.net/api/Timetables/GetRoomTimeTable?id={roomid}&amp;weekDayNum={weekdayNum}</t>
   </si>
 </sst>
 </file>
@@ -98,10 +98,10 @@
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -386,21 +386,21 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:C1"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="95" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="115.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="138.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="31.5" x14ac:dyDescent="0.5">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
@@ -411,19 +411,19 @@
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" t="s">
         <v>3</v>
-      </c>
-      <c r="B4" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>5</v>
+      <c r="A5" s="1" t="s">
+        <v>6</v>
       </c>
       <c r="B5" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
oops, spelled URL wrong.....
</commit_message>
<xml_diff>
--- a/API URLs.xlsx
+++ b/API URLs.xlsx
@@ -41,10 +41,10 @@
     <t>Returns a Json representation of the timetable for the room specified in {roomid} for the day specified by {weekdayNum} (1 = Sunday, 2 = Monday, etc.)</t>
   </si>
   <si>
-    <t>http://signmeinwebapi.azurewebsites.net/api/timetable/{id}</t>
-  </si>
-  <si>
     <t>http://signmeinwebapi.azurewebsites.net/api/Timetables/GetRoomTimeTable?id={roomid}&amp;weekDayNum={weekdayNum}</t>
+  </si>
+  <si>
+    <t>http://signmeinwebapi.azurewebsites.net/api/timetables/{id}</t>
   </si>
 </sst>
 </file>
@@ -386,7 +386,7 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -412,7 +412,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B4" t="s">
         <v>3</v>
@@ -420,7 +420,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B5" t="s">
         <v>4</v>

</xml_diff>